<commit_message>
added and updated some templates
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/sri_lanka/model_input_variables_sri_lanka_se_calibrated.xlsx
+++ b/ref/ingestion/calibrated/sri_lanka/model_input_variables_sri_lanka_se_calibrated.xlsx
@@ -8,16 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
-    <sheet name="strategy_id-5004" sheetId="2" r:id="rId2"/>
-    <sheet name="strategy_id-5007" sheetId="3" r:id="rId3"/>
-    <sheet name="strategy_id-5009" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>subsector</t>
   </si>
@@ -1085,112 +1082,112 @@
         <v>1</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="V6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="X6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Z6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AA6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AB6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AC6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AD6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AE6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AF6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AG6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AH6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AI6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AJ6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AK6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AL6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AM6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AN6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AO6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AP6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AQ6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AR6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AS6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:45">
@@ -1923,822 +1920,6 @@
       </c>
       <c r="AS12">
         <v>6992306.196</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1">
-        <v>9</v>
-      </c>
-      <c r="T1" s="1">
-        <v>10</v>
-      </c>
-      <c r="U1" s="1">
-        <v>11</v>
-      </c>
-      <c r="V1" s="1">
-        <v>12</v>
-      </c>
-      <c r="W1" s="1">
-        <v>13</v>
-      </c>
-      <c r="X1" s="1">
-        <v>14</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="1">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="1">
-        <v>20</v>
-      </c>
-      <c r="AE1" s="1">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="1">
-        <v>22</v>
-      </c>
-      <c r="AG1" s="1">
-        <v>23</v>
-      </c>
-      <c r="AH1" s="1">
-        <v>24</v>
-      </c>
-      <c r="AI1" s="1">
-        <v>25</v>
-      </c>
-      <c r="AJ1" s="1">
-        <v>26</v>
-      </c>
-      <c r="AK1" s="1">
-        <v>27</v>
-      </c>
-      <c r="AL1" s="1">
-        <v>28</v>
-      </c>
-      <c r="AM1" s="1">
-        <v>29</v>
-      </c>
-      <c r="AN1" s="1">
-        <v>30</v>
-      </c>
-      <c r="AO1" s="1">
-        <v>31</v>
-      </c>
-      <c r="AP1" s="1">
-        <v>32</v>
-      </c>
-      <c r="AQ1" s="1">
-        <v>33</v>
-      </c>
-      <c r="AR1" s="1">
-        <v>34</v>
-      </c>
-      <c r="AS1" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>0.98</v>
-      </c>
-      <c r="V2">
-        <v>0.9600000000000001</v>
-      </c>
-      <c r="W2">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="X2">
-        <v>0.9199999999999999</v>
-      </c>
-      <c r="Y2">
-        <v>0.9</v>
-      </c>
-      <c r="Z2">
-        <v>0.88</v>
-      </c>
-      <c r="AA2">
-        <v>0.86</v>
-      </c>
-      <c r="AB2">
-        <v>0.84</v>
-      </c>
-      <c r="AC2">
-        <v>0.8200000000000001</v>
-      </c>
-      <c r="AD2">
-        <v>0.8</v>
-      </c>
-      <c r="AE2">
-        <v>0.78</v>
-      </c>
-      <c r="AF2">
-        <v>0.76</v>
-      </c>
-      <c r="AG2">
-        <v>0.74</v>
-      </c>
-      <c r="AH2">
-        <v>0.72</v>
-      </c>
-      <c r="AI2">
-        <v>0.7</v>
-      </c>
-      <c r="AJ2">
-        <v>0.6799999999999999</v>
-      </c>
-      <c r="AK2">
-        <v>0.6599999999999999</v>
-      </c>
-      <c r="AL2">
-        <v>0.64</v>
-      </c>
-      <c r="AM2">
-        <v>0.62</v>
-      </c>
-      <c r="AN2">
-        <v>0.6</v>
-      </c>
-      <c r="AO2">
-        <v>0.5800000000000001</v>
-      </c>
-      <c r="AP2">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="AQ2">
-        <v>0.54</v>
-      </c>
-      <c r="AR2">
-        <v>0.52</v>
-      </c>
-      <c r="AS2">
-        <v>0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1">
-        <v>9</v>
-      </c>
-      <c r="T1" s="1">
-        <v>10</v>
-      </c>
-      <c r="U1" s="1">
-        <v>11</v>
-      </c>
-      <c r="V1" s="1">
-        <v>12</v>
-      </c>
-      <c r="W1" s="1">
-        <v>13</v>
-      </c>
-      <c r="X1" s="1">
-        <v>14</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="1">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="1">
-        <v>20</v>
-      </c>
-      <c r="AE1" s="1">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="1">
-        <v>22</v>
-      </c>
-      <c r="AG1" s="1">
-        <v>23</v>
-      </c>
-      <c r="AH1" s="1">
-        <v>24</v>
-      </c>
-      <c r="AI1" s="1">
-        <v>25</v>
-      </c>
-      <c r="AJ1" s="1">
-        <v>26</v>
-      </c>
-      <c r="AK1" s="1">
-        <v>27</v>
-      </c>
-      <c r="AL1" s="1">
-        <v>28</v>
-      </c>
-      <c r="AM1" s="1">
-        <v>29</v>
-      </c>
-      <c r="AN1" s="1">
-        <v>30</v>
-      </c>
-      <c r="AO1" s="1">
-        <v>31</v>
-      </c>
-      <c r="AP1" s="1">
-        <v>32</v>
-      </c>
-      <c r="AQ1" s="1">
-        <v>33</v>
-      </c>
-      <c r="AR1" s="1">
-        <v>34</v>
-      </c>
-      <c r="AS1" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>0.98</v>
-      </c>
-      <c r="V2">
-        <v>0.9600000000000001</v>
-      </c>
-      <c r="W2">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="X2">
-        <v>0.9199999999999999</v>
-      </c>
-      <c r="Y2">
-        <v>0.9</v>
-      </c>
-      <c r="Z2">
-        <v>0.88</v>
-      </c>
-      <c r="AA2">
-        <v>0.86</v>
-      </c>
-      <c r="AB2">
-        <v>0.84</v>
-      </c>
-      <c r="AC2">
-        <v>0.8200000000000001</v>
-      </c>
-      <c r="AD2">
-        <v>0.8</v>
-      </c>
-      <c r="AE2">
-        <v>0.78</v>
-      </c>
-      <c r="AF2">
-        <v>0.76</v>
-      </c>
-      <c r="AG2">
-        <v>0.74</v>
-      </c>
-      <c r="AH2">
-        <v>0.72</v>
-      </c>
-      <c r="AI2">
-        <v>0.7</v>
-      </c>
-      <c r="AJ2">
-        <v>0.6799999999999999</v>
-      </c>
-      <c r="AK2">
-        <v>0.6599999999999999</v>
-      </c>
-      <c r="AL2">
-        <v>0.64</v>
-      </c>
-      <c r="AM2">
-        <v>0.62</v>
-      </c>
-      <c r="AN2">
-        <v>0.6</v>
-      </c>
-      <c r="AO2">
-        <v>0.5800000000000001</v>
-      </c>
-      <c r="AP2">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="AQ2">
-        <v>0.54</v>
-      </c>
-      <c r="AR2">
-        <v>0.52</v>
-      </c>
-      <c r="AS2">
-        <v>0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1">
-        <v>9</v>
-      </c>
-      <c r="T1" s="1">
-        <v>10</v>
-      </c>
-      <c r="U1" s="1">
-        <v>11</v>
-      </c>
-      <c r="V1" s="1">
-        <v>12</v>
-      </c>
-      <c r="W1" s="1">
-        <v>13</v>
-      </c>
-      <c r="X1" s="1">
-        <v>14</v>
-      </c>
-      <c r="Y1" s="1">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="1">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="1">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="1">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="1">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="1">
-        <v>20</v>
-      </c>
-      <c r="AE1" s="1">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="1">
-        <v>22</v>
-      </c>
-      <c r="AG1" s="1">
-        <v>23</v>
-      </c>
-      <c r="AH1" s="1">
-        <v>24</v>
-      </c>
-      <c r="AI1" s="1">
-        <v>25</v>
-      </c>
-      <c r="AJ1" s="1">
-        <v>26</v>
-      </c>
-      <c r="AK1" s="1">
-        <v>27</v>
-      </c>
-      <c r="AL1" s="1">
-        <v>28</v>
-      </c>
-      <c r="AM1" s="1">
-        <v>29</v>
-      </c>
-      <c r="AN1" s="1">
-        <v>30</v>
-      </c>
-      <c r="AO1" s="1">
-        <v>31</v>
-      </c>
-      <c r="AP1" s="1">
-        <v>32</v>
-      </c>
-      <c r="AQ1" s="1">
-        <v>33</v>
-      </c>
-      <c r="AR1" s="1">
-        <v>34</v>
-      </c>
-      <c r="AS1" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>0.98</v>
-      </c>
-      <c r="V2">
-        <v>0.9600000000000001</v>
-      </c>
-      <c r="W2">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="X2">
-        <v>0.9199999999999999</v>
-      </c>
-      <c r="Y2">
-        <v>0.9</v>
-      </c>
-      <c r="Z2">
-        <v>0.88</v>
-      </c>
-      <c r="AA2">
-        <v>0.86</v>
-      </c>
-      <c r="AB2">
-        <v>0.84</v>
-      </c>
-      <c r="AC2">
-        <v>0.8200000000000001</v>
-      </c>
-      <c r="AD2">
-        <v>0.8</v>
-      </c>
-      <c r="AE2">
-        <v>0.78</v>
-      </c>
-      <c r="AF2">
-        <v>0.76</v>
-      </c>
-      <c r="AG2">
-        <v>0.74</v>
-      </c>
-      <c r="AH2">
-        <v>0.72</v>
-      </c>
-      <c r="AI2">
-        <v>0.7</v>
-      </c>
-      <c r="AJ2">
-        <v>0.6799999999999999</v>
-      </c>
-      <c r="AK2">
-        <v>0.6599999999999999</v>
-      </c>
-      <c r="AL2">
-        <v>0.64</v>
-      </c>
-      <c r="AM2">
-        <v>0.62</v>
-      </c>
-      <c r="AN2">
-        <v>0.6</v>
-      </c>
-      <c r="AO2">
-        <v>0.5800000000000001</v>
-      </c>
-      <c r="AP2">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="AQ2">
-        <v>0.54</v>
-      </c>
-      <c r="AR2">
-        <v>0.52</v>
-      </c>
-      <c r="AS2">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>